<commit_message>
Assignment : Checking visibility of pagelinks on Account page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Democart.xlsx
+++ b/src/test/resources/testdata/Democart.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="pagelinks" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>firstname</t>
   </si>
@@ -73,6 +73,48 @@
   </si>
   <si>
     <t>1234567849</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>Edit Account</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Address Book</t>
+  </si>
+  <si>
+    <t>Wish List</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>Downloads</t>
+  </si>
+  <si>
+    <t>Recurring payments</t>
+  </si>
+  <si>
+    <t>Reward Points</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>links</t>
   </si>
 </sst>
 </file>
@@ -427,9 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -517,12 +557,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>